<commit_message>
QRS model now is fully hierarchical
Estimates individual QRS steady values for healthy volunteers
</commit_message>
<xml_diff>
--- a/trial_doses.xlsx
+++ b/trial_doses.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/James/Dropbox/MORU/COVID/Chloroquine Poisoning/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/James/Dropbox/MORU/COVID/Chloroquine Poisoning/Code/Chloroquine-concentration-fatality/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{75AF030C-0576-4446-84BF-7AAAF0B88DD0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D07A989F-B406-6F4A-AEB3-C796BD4D40D4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11980" yWindow="5960" windowWidth="27640" windowHeight="16940" xr2:uid="{6D8CD975-F066-5047-9836-D86529CDD722}"/>
+    <workbookView xWindow="6680" yWindow="3060" windowWidth="34700" windowHeight="16940" xr2:uid="{6D8CD975-F066-5047-9836-D86529CDD722}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1066,11 +1066,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A506A71E-1A0D-6A4E-AB18-AA3485FDFB20}">
   <dimension ref="A1:M59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52:XFD55"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43:XFD43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="135" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -1300,7 +1303,7 @@
         <v>2400</v>
       </c>
       <c r="M6">
-        <f>L6*155/200</f>
+        <f t="shared" ref="M6:M11" si="1">L6*155/200</f>
         <v>1860</v>
       </c>
     </row>
@@ -1339,7 +1342,7 @@
         <v>2400</v>
       </c>
       <c r="M7">
-        <f>L7*155/200</f>
+        <f t="shared" si="1"/>
         <v>1860</v>
       </c>
     </row>
@@ -1379,7 +1382,7 @@
         <v>3200</v>
       </c>
       <c r="M8">
-        <f>L8*155/200</f>
+        <f t="shared" si="1"/>
         <v>2480</v>
       </c>
     </row>
@@ -1418,7 +1421,7 @@
         <v>2400</v>
       </c>
       <c r="M9">
-        <f>L9*155/200</f>
+        <f t="shared" si="1"/>
         <v>1860</v>
       </c>
     </row>
@@ -1457,7 +1460,7 @@
         <v>3200</v>
       </c>
       <c r="M10">
-        <f>L10*155/200</f>
+        <f t="shared" si="1"/>
         <v>2480</v>
       </c>
     </row>
@@ -1496,7 +1499,7 @@
         <v>2400</v>
       </c>
       <c r="M11">
-        <f>L11*155/200</f>
+        <f t="shared" si="1"/>
         <v>1860</v>
       </c>
     </row>
@@ -1648,7 +1651,7 @@
         <v>16800</v>
       </c>
       <c r="M15" s="1">
-        <f t="shared" ref="M15:M22" si="1">L15*155/200</f>
+        <f t="shared" ref="M15:M22" si="2">L15*155/200</f>
         <v>13020</v>
       </c>
     </row>
@@ -1687,7 +1690,7 @@
         <v>2400</v>
       </c>
       <c r="M16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1860</v>
       </c>
     </row>
@@ -1727,7 +1730,7 @@
         <v>4400</v>
       </c>
       <c r="M17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3410</v>
       </c>
     </row>
@@ -1766,7 +1769,7 @@
         <v>3200</v>
       </c>
       <c r="M18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2480</v>
       </c>
     </row>
@@ -1806,7 +1809,7 @@
         <v>2400</v>
       </c>
       <c r="M19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1860</v>
       </c>
     </row>
@@ -1846,7 +1849,7 @@
         <v>2400</v>
       </c>
       <c r="M20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1860</v>
       </c>
     </row>
@@ -1885,7 +1888,7 @@
         <v>8000</v>
       </c>
       <c r="M21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6200</v>
       </c>
     </row>
@@ -1925,7 +1928,7 @@
         <v>2800</v>
       </c>
       <c r="M22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2170</v>
       </c>
     </row>
@@ -2165,7 +2168,7 @@
         <v>4200</v>
       </c>
       <c r="M28">
-        <f t="shared" ref="M28:M39" si="2">L28*155/200</f>
+        <f t="shared" ref="M28:M39" si="3">L28*155/200</f>
         <v>3255</v>
       </c>
     </row>
@@ -2204,7 +2207,7 @@
         <v>1600</v>
       </c>
       <c r="M29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1240</v>
       </c>
     </row>
@@ -2244,7 +2247,7 @@
         <v>4400</v>
       </c>
       <c r="M30">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3410</v>
       </c>
     </row>
@@ -2284,7 +2287,7 @@
         <v>3000</v>
       </c>
       <c r="M31">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2325</v>
       </c>
     </row>
@@ -2327,7 +2330,7 @@
         <v>2400</v>
       </c>
       <c r="M32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1860</v>
       </c>
     </row>
@@ -2367,7 +2370,7 @@
         <v>2400</v>
       </c>
       <c r="M33">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1860</v>
       </c>
     </row>
@@ -2407,7 +2410,7 @@
         <v>4200</v>
       </c>
       <c r="M34">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3255</v>
       </c>
     </row>
@@ -2447,7 +2450,7 @@
         <v>4400</v>
       </c>
       <c r="M35">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3410</v>
       </c>
     </row>
@@ -2487,7 +2490,7 @@
         <v>2400</v>
       </c>
       <c r="M36">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1860</v>
       </c>
     </row>
@@ -2527,7 +2530,7 @@
         <v>2400</v>
       </c>
       <c r="M37">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1860</v>
       </c>
     </row>
@@ -2567,7 +2570,7 @@
         <v>12000</v>
       </c>
       <c r="M38" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>9300</v>
       </c>
     </row>
@@ -2607,7 +2610,7 @@
         <v>3400</v>
       </c>
       <c r="M39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2635</v>
       </c>
     </row>
@@ -2716,48 +2719,48 @@
         <v>4000</v>
       </c>
       <c r="M42">
-        <f t="shared" ref="M42:M51" si="3">L42*155/200</f>
+        <f t="shared" ref="M42:M51" si="4">L42*155/200</f>
         <v>3100</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
+    <row r="43" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C43" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D43" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="E43" t="s">
-        <v>17</v>
-      </c>
-      <c r="F43" t="s">
+      <c r="E43" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F43" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="G43">
+      <c r="G43" s="1">
         <v>400</v>
       </c>
-      <c r="H43">
-        <v>2</v>
-      </c>
-      <c r="I43">
+      <c r="H43" s="1">
+        <v>2</v>
+      </c>
+      <c r="I43" s="1">
         <v>10</v>
       </c>
-      <c r="J43" t="s">
-        <v>19</v>
-      </c>
-      <c r="L43">
-        <f>800*2 + 400+ (400*2*9)</f>
-        <v>9200</v>
-      </c>
-      <c r="M43">
-        <f t="shared" si="3"/>
-        <v>7130</v>
+      <c r="J43" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L43" s="1">
+        <f>800*2 + 400+ (400*2*9) + 400</f>
+        <v>9600</v>
+      </c>
+      <c r="M43" s="1">
+        <f t="shared" si="4"/>
+        <v>7440</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.2">
@@ -2796,7 +2799,7 @@
         <v>2800</v>
       </c>
       <c r="M44">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2170</v>
       </c>
     </row>
@@ -2836,7 +2839,7 @@
         <v>6400</v>
       </c>
       <c r="M45">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4960</v>
       </c>
     </row>
@@ -2876,7 +2879,7 @@
         <v>2000</v>
       </c>
       <c r="M46">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1550</v>
       </c>
     </row>
@@ -2916,7 +2919,7 @@
         <v>4400</v>
       </c>
       <c r="M47">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3410</v>
       </c>
     </row>
@@ -2956,7 +2959,7 @@
         <v>8400</v>
       </c>
       <c r="M48">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>6510</v>
       </c>
     </row>
@@ -2996,7 +2999,7 @@
         <v>2400</v>
       </c>
       <c r="M49">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1860</v>
       </c>
     </row>
@@ -3035,7 +3038,7 @@
         <v>6000</v>
       </c>
       <c r="M50">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4650</v>
       </c>
     </row>
@@ -3075,7 +3078,7 @@
         <v>2400</v>
       </c>
       <c r="M51">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1860</v>
       </c>
     </row>
@@ -3158,7 +3161,7 @@
         <v>5500</v>
       </c>
       <c r="M53">
-        <f t="shared" ref="M53:M59" si="4">L53*155/250</f>
+        <f t="shared" ref="M53:M59" si="5">L53*155/250</f>
         <v>3410</v>
       </c>
     </row>
@@ -3198,7 +3201,7 @@
         <v>8000</v>
       </c>
       <c r="M54">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4960</v>
       </c>
     </row>
@@ -3238,7 +3241,7 @@
         <v>20000</v>
       </c>
       <c r="M55" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>12400</v>
       </c>
     </row>
@@ -3277,7 +3280,7 @@
         <v>7000</v>
       </c>
       <c r="M56">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4340</v>
       </c>
     </row>
@@ -3316,7 +3319,7 @@
         <v>5000</v>
       </c>
       <c r="M57">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3100</v>
       </c>
     </row>
@@ -3356,7 +3359,7 @@
         <v>4400</v>
       </c>
       <c r="M58">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2728</v>
       </c>
     </row>
@@ -3396,7 +3399,7 @@
         <v>3000</v>
       </c>
       <c r="M59">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1860</v>
       </c>
     </row>

</xml_diff>

<commit_message>
mistake in SOLIDARITY dosing
</commit_message>
<xml_diff>
--- a/trial_doses.xlsx
+++ b/trial_doses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/James/Dropbox/MORU/COVID/Chloroquine Poisoning/Code/Chloroquine-concentration-fatality/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F56758FE-DF19-B545-BF0E-13BB14CF4C4C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FD18F74-2D12-764B-924A-BD9CB08C10D3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6680" yWindow="3060" windowWidth="34700" windowHeight="16940" xr2:uid="{6D8CD975-F066-5047-9836-D86529CDD722}"/>
   </bookViews>
@@ -1077,8 +1077,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A506A71E-1A0D-6A4E-AB18-AA3485FDFB20}">
   <dimension ref="A1:M59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1233,17 +1233,17 @@
         <v>2</v>
       </c>
       <c r="I4" s="1">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>19</v>
       </c>
       <c r="L4" s="1">
-        <v>8800</v>
+        <v>9600</v>
       </c>
       <c r="M4" s="1">
         <f t="shared" si="0"/>
-        <v>6820</v>
+        <v>7440</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">

</xml_diff>